<commit_message>
Manually code unstructured data
</commit_message>
<xml_diff>
--- a/chat_exports/df_before_standard.xlsx
+++ b/chat_exports/df_before_standard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,16 +474,6 @@
           <t>q15_price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>q18_important_features</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>q39_contradictory_info</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -522,16 +512,6 @@
           <t>1,359</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>["Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>["Other"]</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -574,16 +554,6 @@
           <t>740</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Display Quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>["I did not find any contradictions"]</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -626,16 +596,6 @@
           <t>600</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Storage capacity","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>["I trusted the first response I got","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -678,16 +638,6 @@
           <t>1200</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Display Quality"]</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>["I did not find any contradictions"]</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -730,16 +680,6 @@
           <t>700</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources"]</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -778,16 +718,6 @@
           <t>I forget</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -828,16 +758,6 @@
       <c r="H8" t="inlineStr">
         <is>
           <t>I don't know</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources"]</t>
         </is>
       </c>
     </row>
@@ -874,16 +794,6 @@
           <t>300</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>["Camera quality"]</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources"]</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -926,16 +836,6 @@
           <t xml:space="preserve">Don’t know </t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>["I did not find any contradictions"]</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -976,16 +876,6 @@
       <c r="H11" t="inlineStr">
         <is>
           <t>839 eur</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>["Camera quality","Performance/ speed","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment"]</t>
         </is>
       </c>
     </row>
@@ -1022,16 +912,6 @@
           <t>€801</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>["Performance/ speed","Camera quality"]</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources"]</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1066,16 +946,6 @@
           <t>208</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>["Performance/ speed","Storage capacity","Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>["Other"]</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1116,16 +986,6 @@
       <c r="H14" t="inlineStr">
         <is>
           <t>630</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>["I trusted the first response I got","I chose the response that seemed most detailed or complete","I relied on my own knowledge or judgment"]</t>
         </is>
       </c>
     </row>
@@ -1162,16 +1022,6 @@
           <t>1023</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1206,16 +1056,6 @@
           <t>€799</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>["Display Quality","Software support &amp; updates","Camera quality"]</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1256,16 +1096,6 @@
       <c r="H17" t="inlineStr">
         <is>
           <t>€1299</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>["Camera quality","Performance/ speed","Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment","I asked more questions or looked for additional sources"]</t>
         </is>
       </c>
     </row>
@@ -1298,16 +1128,6 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Display Quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>["I did not find any contradictions"]</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1342,16 +1162,6 @@
           <t>600</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources"]</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1394,16 +1204,6 @@
           <t>900</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources"]</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1446,16 +1246,6 @@
           <t>650€</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>["Camera quality","Performance/ speed","Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1498,16 +1288,6 @@
           <t>639</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>["Camera quality","Storage capacity","Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1550,16 +1330,6 @@
           <t>119€</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Display Quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1602,16 +1372,6 @@
           <t>702</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>["I chose the response that seemed most detailed or complete","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1654,16 +1414,6 @@
           <t>919</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>["Software support &amp; updates","Battery life/ fast charging","Display Quality"]</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1706,16 +1456,6 @@
           <t>€1039</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>["Camera quality","Performance/ speed","Battery life/ fast charging"]</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I chose the response that seemed most detailed or complete","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1758,16 +1498,6 @@
           <t>€799</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>["Performance/ speed","Storage capacity","Battery life/ fast charging"]</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1808,16 +1538,6 @@
       <c r="H28" t="inlineStr">
         <is>
           <t>399</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources"]</t>
         </is>
       </c>
     </row>
@@ -1854,16 +1574,6 @@
           <t xml:space="preserve">No idea </t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1906,16 +1616,6 @@
           <t>€377.99</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>["Display Quality","Software support &amp; updates","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources"]</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1958,16 +1658,6 @@
           <t>350</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Display Quality"]</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>["I trusted the first response I got","I chose the response that seemed most detailed or complete","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2010,16 +1700,6 @@
           <t>1065</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>["Camera quality","Display Quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>["I chose the response that seemed most detailed or complete"]</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2062,16 +1742,6 @@
           <t>168.8</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Performance/ speed","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2114,16 +1784,6 @@
           <t>299</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>["I did not find any contradictions"]</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2166,16 +1826,6 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Display Quality","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2216,16 +1866,6 @@
       <c r="H36" t="inlineStr">
         <is>
           <t>~€380</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Storage capacity","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I relied on my own knowledge or judgment"]</t>
         </is>
       </c>
     </row>
@@ -2262,16 +1902,6 @@
           <t>799</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>["Display Quality","Performance/ speed","Storage capacity"]</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I chose the response that seemed most detailed or complete","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2314,16 +1944,6 @@
           <t>749 euros</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging"]</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>["I trusted the first response I got"]</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2360,16 +1980,6 @@
       <c r="H39" t="inlineStr">
         <is>
           <t>559</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>["I trusted the first response I got"]</t>
         </is>
       </c>
     </row>
@@ -2406,16 +2016,6 @@
           <t>Approximately €800</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Other"]</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>["I did not find any contradictions"]</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2458,16 +2058,6 @@
           <t>1299</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>["Software support &amp; updates","Storage capacity","Battery life/ fast charging"]</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2510,16 +2100,6 @@
           <t>1167,38€ ( for new one )</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>["I asked more questions or looked for additional sources","I chose the response that seemed most detailed or complete"]</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2558,16 +2138,6 @@
           <t>444 €</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Performance/ speed","Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>["I trusted the first response I got","I chose the response that seemed most detailed or complete","I relied on my own knowledge or judgment"]</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2606,16 +2176,6 @@
           <t>€336.55</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Display Quality"]</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>["I trusted the first response I got","I did not find any contradictions"]</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2658,16 +2218,6 @@
           <t>699</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>["Camera quality","Performance/ speed","Software support &amp; updates"]</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment","I did not find any contradictions"]</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2708,16 +2258,6 @@
       <c r="H46" t="inlineStr">
         <is>
           <t>1000</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>["Battery life/ fast charging","Camera quality","Performance/ speed"]</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>["I relied on my own knowledge or judgment"]</t>
         </is>
       </c>
     </row>

</xml_diff>